<commit_message>
src: routes: - updated the csv import
</commit_message>
<xml_diff>
--- a/templates/user_template.xlsx
+++ b/templates/user_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gitRepo\siba-be\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2AD3C76-9F83-4B56-9983-6385D3562D62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B6E635-F79E-41F3-8015-1D73568BEC14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="11235" xr2:uid="{62F6EE3A-6D08-43A2-9CB6-016DBF45EA6C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{62F6EE3A-6D08-43A2-9CB6-016DBF45EA6C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -77,7 +77,7 @@
     <t>add 0 or 1</t>
   </si>
   <si>
-    <t>name of department 1/name of department 2</t>
+    <t>name of department 1|name of department 2</t>
   </si>
 </sst>
 </file>
@@ -478,7 +478,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>